<commit_message>
fix: shift import to all
</commit_message>
<xml_diff>
--- a/AccuPay/ImportTemplates/accupay-shiftschedule-template.xlsx
+++ b/AccuPay/ImportTemplates/accupay-shiftschedule-template.xlsx
@@ -200,7 +200,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -241,6 +241,8 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -250,7 +252,6 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma 2" xfId="1"/>
@@ -548,31 +549,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
       <c r="F1" s="4"/>
     </row>
     <row r="3" spans="1:6" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="31"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
+      <c r="A4" s="33"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
     </row>
     <row r="6" spans="1:6" s="11" customFormat="1">
       <c r="A6" s="7" t="s">
@@ -718,20 +719,22 @@
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" style="14" customWidth="1"/>
+    <col min="1" max="1" width="89.7109375" style="14" customWidth="1"/>
     <col min="2" max="2" width="18.7109375" style="15" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" style="15" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" style="31" hidden="1" customWidth="1"/>
     <col min="4" max="5" width="10.42578125" style="16" customWidth="1"/>
     <col min="6" max="6" width="25.5703125" style="16" customWidth="1"/>
     <col min="7" max="7" width="22.42578125" style="17" customWidth="1"/>
     <col min="8" max="8" width="26.28515625" style="14" customWidth="1"/>
-    <col min="9" max="9" width="0" style="33" hidden="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="33"/>
+    <col min="9" max="9" width="15.5703125" style="30" hidden="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="30"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -759,12 +762,12 @@
       <c r="H1" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="33" t="s">
+      <c r="I1" s="30" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="r3UmekJ/tEefQpNGyA2c2Sv9tx3DXuRNE7j7A/7vBAVH/5iQN6QOpK7i+9axsbXXy9AYcxJEaNkT7ukVxpadbw==" saltValue="Vu9L45x3uQhZ8iKQCvtQ9A==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="yFsnhkAp27suZtr99WKtysvRBwRcnv8PYiGIi7JUOCZc+iWVXnrjBbO6nVOQMhe7NEs/uagtKnaf1K7GZVJj9w==" saltValue="oSv4etJijTlsGAxZCXczug==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
@@ -791,16 +794,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
@@ -834,11 +837,11 @@
       </c>
       <c r="B3" s="28">
         <f ca="1">TODAY()+(7-WEEKDAY(TODAY(),2)+1)</f>
-        <v>45012</v>
+        <v>45033</v>
       </c>
       <c r="C3" s="25">
         <f ca="1">TODAY()+(7-WEEKDAY(TODAY(),2)+5)</f>
-        <v>45016</v>
+        <v>45037</v>
       </c>
       <c r="D3" s="26">
         <v>0.33333333333333298</v>
@@ -859,7 +862,7 @@
       </c>
       <c r="B4" s="25">
         <f ca="1">TODAY()+(7-WEEKDAY(TODAY(),2)+6)</f>
-        <v>45017</v>
+        <v>45038</v>
       </c>
       <c r="D4" s="26">
         <v>0.29166666666666702</v>
@@ -880,11 +883,11 @@
       </c>
       <c r="B5" s="25">
         <f ca="1">TODAY()+(7-WEEKDAY(TODAY(),2)+8)</f>
-        <v>45019</v>
+        <v>45040</v>
       </c>
       <c r="C5" s="25">
         <f ca="1">TODAY()+(7-WEEKDAY(TODAY(),2)+11)</f>
-        <v>45022</v>
+        <v>45043</v>
       </c>
       <c r="D5" s="26">
         <v>0.875</v>
@@ -905,7 +908,7 @@
       </c>
       <c r="B6" s="25">
         <f ca="1">TODAY()+(7-WEEKDAY(TODAY(),2)+12)</f>
-        <v>45023</v>
+        <v>45044</v>
       </c>
       <c r="H6" s="29" t="s">
         <v>28</v>
@@ -917,11 +920,11 @@
       </c>
       <c r="B7" s="25">
         <f ca="1">TODAY()+(7-WEEKDAY(TODAY(),2)+13)</f>
-        <v>45024</v>
+        <v>45045</v>
       </c>
       <c r="C7" s="25">
         <f ca="1">TODAY()+(7-WEEKDAY(TODAY(),2)+14)</f>
-        <v>45025</v>
+        <v>45046</v>
       </c>
       <c r="D7" s="26">
         <v>0.625</v>

</xml_diff>